<commit_message>
updates for 5-24 Leadership Institute class
</commit_message>
<xml_diff>
--- a/Labs/Lab 2 Assets/Lab 2 - midpoint.xlsx
+++ b/Labs/Lab 2 Assets/Lab 2 - midpoint.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias\Desktop\LI_Local\Labs\Lab 2 Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\LI Data\Class\Labs\Lab 2 Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="9860"/>
   </bookViews>
   <sheets>
-    <sheet name="Jobs By State" sheetId="4" r:id="rId1"/>
+    <sheet name="Jobs by State" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,14 +35,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,15 +77,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -102,7 +125,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -114,7 +137,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -131,9 +154,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -161,14 +184,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -196,6 +236,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -348,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C247"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -368,10 +425,10 @@
       <c r="A2" s="1">
         <v>38353</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>16439418</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>10429794</v>
       </c>
     </row>
@@ -379,10 +436,10 @@
       <c r="A3" s="1">
         <v>38384</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>16465728</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>10448959</v>
       </c>
     </row>
@@ -390,10 +447,10 @@
       <c r="A4" s="1">
         <v>38412</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>16496882</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>10469293</v>
       </c>
     </row>
@@ -401,10 +458,10 @@
       <c r="A5" s="1">
         <v>38443</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>16532483</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>10490555</v>
       </c>
     </row>
@@ -412,10 +469,10 @@
       <c r="A6" s="1">
         <v>38473</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>16570179</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>10513096</v>
       </c>
     </row>
@@ -423,10 +480,10 @@
       <c r="A7" s="1">
         <v>38504</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>16604314</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>10535779</v>
       </c>
     </row>
@@ -434,10 +491,10 @@
       <c r="A8" s="1">
         <v>38534</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>16629998</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>10557004</v>
       </c>
     </row>
@@ -445,10 +502,10 @@
       <c r="A9" s="1">
         <v>38565</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>16646101</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>10576195</v>
       </c>
     </row>
@@ -456,10 +513,10 @@
       <c r="A10" s="1">
         <v>38596</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>16654448</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>10593587</v>
       </c>
     </row>
@@ -467,10 +524,10 @@
       <c r="A11" s="1">
         <v>38626</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>16659074</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>10609861</v>
       </c>
     </row>
@@ -478,10 +535,10 @@
       <c r="A12" s="1">
         <v>38657</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>16663192</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>10625255</v>
       </c>
     </row>
@@ -489,10 +546,10 @@
       <c r="A13" s="1">
         <v>38687</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>16668652</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>10639901</v>
       </c>
     </row>
@@ -500,10 +557,10 @@
       <c r="A14" s="1">
         <v>38718</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>16678345</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>10654741</v>
       </c>
     </row>
@@ -511,10 +568,10 @@
       <c r="A15" s="1">
         <v>38749</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>16692767</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>10670407</v>
       </c>
     </row>
@@ -522,10 +579,10 @@
       <c r="A16" s="1">
         <v>38777</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>16709821</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>10687000</v>
       </c>
     </row>
@@ -533,10 +590,10 @@
       <c r="A17" s="1">
         <v>38808</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>16727112</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>10704217</v>
       </c>
     </row>
@@ -544,10 +601,10 @@
       <c r="A18" s="1">
         <v>38838</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>16744724</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>10722253</v>
       </c>
     </row>
@@ -555,10 +612,10 @@
       <c r="A19" s="1">
         <v>38869</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>16763184</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>10741372</v>
       </c>
     </row>
@@ -566,10 +623,10 @@
       <c r="A20" s="1">
         <v>38899</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>16784652</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>10762673</v>
       </c>
     </row>
@@ -577,10 +634,10 @@
       <c r="A21" s="1">
         <v>38930</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>16809465</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>10785501</v>
       </c>
     </row>
@@ -588,10 +645,10 @@
       <c r="A22" s="1">
         <v>38961</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>16836006</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>10807990</v>
       </c>
     </row>
@@ -599,10 +656,10 @@
       <c r="A23" s="1">
         <v>38991</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>16863434</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>10828643</v>
       </c>
     </row>
@@ -610,10 +667,10 @@
       <c r="A24" s="1">
         <v>39022</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>16888929</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>10845617</v>
       </c>
     </row>
@@ -621,10 +678,10 @@
       <c r="A25" s="1">
         <v>39052</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>16908652</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>10857679</v>
       </c>
     </row>
@@ -632,10 +689,10 @@
       <c r="A26" s="1">
         <v>39083</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>16919913</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>10865076</v>
       </c>
     </row>
@@ -643,10 +700,10 @@
       <c r="A27" s="1">
         <v>39114</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>16924066</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3">
         <v>10869826</v>
       </c>
     </row>
@@ -654,10 +711,10 @@
       <c r="A28" s="1">
         <v>39142</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>16924161</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>10873929</v>
       </c>
     </row>
@@ -665,10 +722,10 @@
       <c r="A29" s="1">
         <v>39173</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>16923640</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <v>10879363</v>
       </c>
     </row>
@@ -676,10 +733,10 @@
       <c r="A30" s="1">
         <v>39203</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>16923972</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3">
         <v>10887203</v>
       </c>
     </row>
@@ -687,10 +744,10 @@
       <c r="A31" s="1">
         <v>39234</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>16925738</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3">
         <v>10897836</v>
       </c>
     </row>
@@ -698,10 +755,10 @@
       <c r="A32" s="1">
         <v>39264</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>16928751</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3">
         <v>10911124</v>
       </c>
     </row>
@@ -709,10 +766,10 @@
       <c r="A33" s="1">
         <v>39295</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>16932459</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3">
         <v>10926733</v>
       </c>
     </row>
@@ -720,10 +777,10 @@
       <c r="A34" s="1">
         <v>39326</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>16937003</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3">
         <v>10944308</v>
       </c>
     </row>
@@ -731,10 +788,10 @@
       <c r="A35" s="1">
         <v>39356</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>16941177</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="3">
         <v>10962541</v>
       </c>
     </row>
@@ -742,10 +799,10 @@
       <c r="A36" s="1">
         <v>39387</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>16944750</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="3">
         <v>10980429</v>
       </c>
     </row>
@@ -753,10 +810,10 @@
       <c r="A37" s="1">
         <v>39417</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>16948344</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="3">
         <v>10997356</v>
       </c>
     </row>
@@ -764,10 +821,10 @@
       <c r="A38" s="1">
         <v>39448</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>16949786</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="3">
         <v>11012517</v>
       </c>
     </row>
@@ -775,10 +832,10 @@
       <c r="A39" s="1">
         <v>39479</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <v>16947111</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>11026440</v>
       </c>
     </row>
@@ -786,10 +843,10 @@
       <c r="A40" s="1">
         <v>39508</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>16938974</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <v>11039924</v>
       </c>
     </row>
@@ -797,10 +854,10 @@
       <c r="A41" s="1">
         <v>39539</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>16925829</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="3">
         <v>11053331</v>
       </c>
     </row>
@@ -808,10 +865,10 @@
       <c r="A42" s="1">
         <v>39569</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>16909310</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="3">
         <v>11066349</v>
       </c>
     </row>
@@ -819,10 +876,10 @@
       <c r="A43" s="1">
         <v>39600</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <v>16890998</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="3">
         <v>11078197</v>
       </c>
     </row>
@@ -830,10 +887,10 @@
       <c r="A44" s="1">
         <v>39630</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="2">
         <v>16869946</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="3">
         <v>11087308</v>
       </c>
     </row>
@@ -841,10 +898,10 @@
       <c r="A45" s="1">
         <v>39661</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <v>16843619</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="3">
         <v>11092047</v>
       </c>
     </row>
@@ -852,10 +909,10 @@
       <c r="A46" s="1">
         <v>39692</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="2">
         <v>16807462</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="3">
         <v>11091066</v>
       </c>
     </row>
@@ -863,10 +920,10 @@
       <c r="A47" s="1">
         <v>39722</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="2">
         <v>16757144</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="3">
         <v>11084099</v>
       </c>
     </row>
@@ -874,10 +931,10 @@
       <c r="A48" s="1">
         <v>39753</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="2">
         <v>16690415</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="3">
         <v>11072158</v>
       </c>
     </row>
@@ -885,10 +942,10 @@
       <c r="A49" s="1">
         <v>39783</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="2">
         <v>16608946</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="3">
         <v>11057807</v>
       </c>
     </row>
@@ -896,10 +953,10 @@
       <c r="A50" s="1">
         <v>39814</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="2">
         <v>16519067</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="3">
         <v>11044551</v>
       </c>
     </row>
@@ -907,10 +964,10 @@
       <c r="A51" s="1">
         <v>39845</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="2">
         <v>16429442</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="3">
         <v>11035607</v>
       </c>
     </row>
@@ -918,10 +975,10 @@
       <c r="A52" s="1">
         <v>39873</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="2">
         <v>16348527</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="3">
         <v>11033021</v>
       </c>
     </row>
@@ -929,10 +986,10 @@
       <c r="A53" s="1">
         <v>39904</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="2">
         <v>16279164</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="3">
         <v>11035856</v>
       </c>
     </row>
@@ -940,10 +997,10 @@
       <c r="A54" s="1">
         <v>39934</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="2">
         <v>16218134</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="3">
         <v>11040565</v>
       </c>
     </row>
@@ -951,10 +1008,10 @@
       <c r="A55" s="1">
         <v>39965</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="2">
         <v>16162381</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="3">
         <v>11044463</v>
       </c>
     </row>
@@ -962,10 +1019,10 @@
       <c r="A56" s="1">
         <v>39995</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="2">
         <v>16109437</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="3">
         <v>11045916</v>
       </c>
     </row>
@@ -973,10 +1030,10 @@
       <c r="A57" s="1">
         <v>40026</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="2">
         <v>16059591</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="3">
         <v>11045998</v>
       </c>
     </row>
@@ -984,10 +1041,10 @@
       <c r="A58" s="1">
         <v>40057</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="2">
         <v>16016763</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="3">
         <v>11048293</v>
       </c>
     </row>
@@ -995,10 +1052,10 @@
       <c r="A59" s="1">
         <v>40087</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="2">
         <v>15984660</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="3">
         <v>11056133</v>
       </c>
     </row>
@@ -1006,10 +1063,10 @@
       <c r="A60" s="1">
         <v>40118</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="2">
         <v>15968221</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="3">
         <v>11072710</v>
       </c>
     </row>
@@ -1017,10 +1074,10 @@
       <c r="A61" s="1">
         <v>40148</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="2">
         <v>15970426</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="3">
         <v>11098518</v>
       </c>
     </row>
@@ -1028,10 +1085,10 @@
       <c r="A62" s="1">
         <v>40179</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="2">
         <v>15990075</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="3">
         <v>11131072</v>
       </c>
     </row>
@@ -1039,10 +1096,10 @@
       <c r="A63" s="1">
         <v>40210</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="2">
         <v>16020752</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="3">
         <v>11165726</v>
       </c>
     </row>
@@ -1050,10 +1107,10 @@
       <c r="A64" s="1">
         <v>40238</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="2">
         <v>16054668</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="3">
         <v>11198527</v>
       </c>
     </row>
@@ -1061,10 +1118,10 @@
       <c r="A65" s="1">
         <v>40269</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="2">
         <v>16085283</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="3">
         <v>11227360</v>
       </c>
     </row>
@@ -1072,10 +1129,10 @@
       <c r="A66" s="1">
         <v>40299</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="2">
         <v>16108007</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="3">
         <v>11251801</v>
       </c>
     </row>
@@ -1083,10 +1140,10 @@
       <c r="A67" s="1">
         <v>40330</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="2">
         <v>16118626</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="3">
         <v>11272121</v>
       </c>
     </row>
@@ -1094,10 +1151,10 @@
       <c r="A68" s="1">
         <v>40360</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="2">
         <v>16117151</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="3">
         <v>11289821</v>
       </c>
     </row>
@@ -1105,10 +1162,10 @@
       <c r="A69" s="1">
         <v>40391</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="2">
         <v>16108665</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="3">
         <v>11307188</v>
       </c>
     </row>
@@ -1116,10 +1173,10 @@
       <c r="A70" s="1">
         <v>40422</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="2">
         <v>16098748</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="3">
         <v>11325265</v>
       </c>
     </row>
@@ -1127,10 +1184,10 @@
       <c r="A71" s="1">
         <v>40452</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="2">
         <v>16093821</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="3">
         <v>11345452</v>
       </c>
     </row>
@@ -1138,10 +1195,10 @@
       <c r="A72" s="1">
         <v>40483</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="2">
         <v>16096865</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="3">
         <v>11367749</v>
       </c>
     </row>
@@ -1149,10 +1206,10 @@
       <c r="A73" s="1">
         <v>40513</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="2">
         <v>16106822</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="3">
         <v>11391102</v>
       </c>
     </row>
@@ -1160,939 +1217,837 @@
       <c r="A74" s="1">
         <v>40544</v>
       </c>
-      <c r="B74">
-        <v>16121358</v>
-      </c>
-      <c r="C74">
-        <v>11414526</v>
+      <c r="B74" s="2">
+        <v>16126436</v>
+      </c>
+      <c r="C74" s="3">
+        <v>11414646</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>40575</v>
       </c>
-      <c r="B75">
-        <v>16136717</v>
-      </c>
-      <c r="C75">
-        <v>11436373</v>
+      <c r="B75" s="2">
+        <v>16142486</v>
+      </c>
+      <c r="C75" s="3">
+        <v>11436424</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>40603</v>
       </c>
-      <c r="B76">
-        <v>16149958</v>
-      </c>
-      <c r="C76">
-        <v>11455953</v>
+      <c r="B76" s="2">
+        <v>16156123</v>
+      </c>
+      <c r="C76" s="3">
+        <v>11455656</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>40634</v>
       </c>
-      <c r="B77">
-        <v>16161275</v>
-      </c>
-      <c r="C77">
-        <v>11473960</v>
+      <c r="B77" s="2">
+        <v>16167337</v>
+      </c>
+      <c r="C77" s="3">
+        <v>11472999</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>40664</v>
       </c>
-      <c r="B78">
-        <v>16174607</v>
-      </c>
-      <c r="C78">
-        <v>11492586</v>
+      <c r="B78" s="2">
+        <v>16180189</v>
+      </c>
+      <c r="C78" s="3">
+        <v>11490846</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>40695</v>
       </c>
-      <c r="B79">
-        <v>16194872</v>
-      </c>
-      <c r="C79">
-        <v>11514157</v>
+      <c r="B79" s="2">
+        <v>16199980</v>
+      </c>
+      <c r="C79" s="3">
+        <v>11511881</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>40725</v>
       </c>
-      <c r="B80">
-        <v>16224712</v>
-      </c>
-      <c r="C80">
-        <v>11539959</v>
+      <c r="B80" s="2">
+        <v>16230013</v>
+      </c>
+      <c r="C80" s="3">
+        <v>11537804</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>40756</v>
       </c>
-      <c r="B81">
-        <v>16261868</v>
-      </c>
-      <c r="C81">
-        <v>11569179</v>
+      <c r="B81" s="2">
+        <v>16268316</v>
+      </c>
+      <c r="C81" s="3">
+        <v>11567820</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>40787</v>
       </c>
-      <c r="B82">
-        <v>16301692</v>
-      </c>
-      <c r="C82">
-        <v>11599833</v>
+      <c r="B82" s="2">
+        <v>16310009</v>
+      </c>
+      <c r="C82" s="3">
+        <v>11599685</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>40817</v>
       </c>
-      <c r="B83">
-        <v>16339543</v>
-      </c>
-      <c r="C83">
-        <v>11629859</v>
+      <c r="B83" s="2">
+        <v>16350024</v>
+      </c>
+      <c r="C83" s="3">
+        <v>11630888</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>40848</v>
       </c>
-      <c r="B84">
-        <v>16371250</v>
-      </c>
-      <c r="C84">
-        <v>11657488</v>
+      <c r="B84" s="2">
+        <v>16383739</v>
+      </c>
+      <c r="C84" s="3">
+        <v>11659190</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>40878</v>
       </c>
-      <c r="B85">
-        <v>16395681</v>
-      </c>
-      <c r="C85">
-        <v>11682375</v>
+      <c r="B85" s="2">
+        <v>16409743</v>
+      </c>
+      <c r="C85" s="3">
+        <v>11683975</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>40909</v>
       </c>
-      <c r="B86">
-        <v>16415566</v>
-      </c>
-      <c r="C86">
-        <v>11705210</v>
+      <c r="B86" s="2">
+        <v>16410566</v>
+      </c>
+      <c r="C86" s="3">
+        <v>11706359</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>40940</v>
       </c>
-      <c r="B87">
-        <v>16435399</v>
-      </c>
-      <c r="C87">
-        <v>11727071</v>
+      <c r="B87" s="2">
+        <v>16429555</v>
+      </c>
+      <c r="C87" s="3">
+        <v>11725922</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>40969</v>
       </c>
-      <c r="B88">
-        <v>16457451</v>
-      </c>
-      <c r="C88">
-        <v>11748416</v>
+      <c r="B88" s="2">
+        <v>16450378</v>
+      </c>
+      <c r="C88" s="3">
+        <v>11744571</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>41000</v>
       </c>
-      <c r="B89">
-        <v>16482198</v>
-      </c>
-      <c r="C89">
-        <v>11770028</v>
+      <c r="B89" s="2">
+        <v>16474446</v>
+      </c>
+      <c r="C89" s="3">
+        <v>11763538</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>41030</v>
       </c>
-      <c r="B90">
-        <v>16511414</v>
-      </c>
-      <c r="C90">
-        <v>11793629</v>
+      <c r="B90" s="2">
+        <v>16504046</v>
+      </c>
+      <c r="C90" s="3">
+        <v>11785438</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>41061</v>
       </c>
-      <c r="B91">
-        <v>16546749</v>
-      </c>
-      <c r="C91">
-        <v>11819750</v>
+      <c r="B91" s="2">
+        <v>16540349</v>
+      </c>
+      <c r="C91" s="3">
+        <v>11811338</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>41091</v>
       </c>
-      <c r="B92">
-        <v>16588860</v>
-      </c>
-      <c r="C92">
-        <v>11847476</v>
+      <c r="B92" s="2">
+        <v>16583277</v>
+      </c>
+      <c r="C92" s="3">
+        <v>11840381</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>41122</v>
       </c>
-      <c r="B93">
-        <v>16636523</v>
-      </c>
-      <c r="C93">
-        <v>11875135</v>
+      <c r="B93" s="2">
+        <v>16630757</v>
+      </c>
+      <c r="C93" s="3">
+        <v>11869933</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>41153</v>
       </c>
-      <c r="B94">
-        <v>16687351</v>
-      </c>
-      <c r="C94">
-        <v>11901218</v>
+      <c r="B94" s="2">
+        <v>16679801</v>
+      </c>
+      <c r="C94" s="3">
+        <v>11897067</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>41183</v>
       </c>
-      <c r="B95">
-        <v>16737374</v>
-      </c>
-      <c r="C95">
-        <v>11924467</v>
+      <c r="B95" s="2">
+        <v>16725935</v>
+      </c>
+      <c r="C95" s="3">
+        <v>11918880</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>41214</v>
       </c>
-      <c r="B96">
-        <v>16783601</v>
-      </c>
-      <c r="C96">
-        <v>11944993</v>
+      <c r="B96" s="2">
+        <v>16766410</v>
+      </c>
+      <c r="C96" s="3">
+        <v>11934926</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>41244</v>
       </c>
-      <c r="B97">
-        <v>16824921</v>
-      </c>
-      <c r="C97">
-        <v>11964225</v>
+      <c r="B97" s="2">
+        <v>16801207</v>
+      </c>
+      <c r="C97" s="3">
+        <v>11947373</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>41275</v>
       </c>
-      <c r="B98">
-        <v>16860099</v>
-      </c>
-      <c r="C98">
-        <v>11983739</v>
+      <c r="B98" s="2">
+        <v>16830800</v>
+      </c>
+      <c r="C98" s="3">
+        <v>11959311</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>41306</v>
       </c>
-      <c r="B99">
-        <v>16890116</v>
-      </c>
-      <c r="C99">
-        <v>12005178</v>
+      <c r="B99" s="2">
+        <v>16857321</v>
+      </c>
+      <c r="C99" s="3">
+        <v>11974552</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>41334</v>
       </c>
-      <c r="B100">
-        <v>16918326</v>
-      </c>
-      <c r="C100">
-        <v>12029227</v>
+      <c r="B100" s="2">
+        <v>16883994</v>
+      </c>
+      <c r="C100" s="3">
+        <v>11995524</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>41365</v>
       </c>
-      <c r="B101">
-        <v>16947599</v>
-      </c>
-      <c r="C101">
-        <v>12055117</v>
+      <c r="B101" s="2">
+        <v>16912823</v>
+      </c>
+      <c r="C101" s="3">
+        <v>12021947</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>41395</v>
       </c>
-      <c r="B102">
-        <v>16975365</v>
-      </c>
-      <c r="C102">
-        <v>12080207</v>
+      <c r="B102" s="2">
+        <v>16939922</v>
+      </c>
+      <c r="C102" s="3">
+        <v>12049253</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>41426</v>
       </c>
-      <c r="B103">
-        <v>16998744</v>
-      </c>
-      <c r="C103">
-        <v>12103390</v>
+      <c r="B103" s="2">
+        <v>16962014</v>
+      </c>
+      <c r="C103" s="3">
+        <v>12073991</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>41456</v>
       </c>
-      <c r="B104">
-        <v>17017749</v>
-      </c>
-      <c r="C104">
-        <v>12126081</v>
+      <c r="B104" s="2">
+        <v>16978808</v>
+      </c>
+      <c r="C104" s="3">
+        <v>12095358</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>41487</v>
       </c>
-      <c r="B105">
-        <v>17034487</v>
-      </c>
-      <c r="C105">
-        <v>12150156</v>
+      <c r="B105" s="2">
+        <v>16992571</v>
+      </c>
+      <c r="C105" s="3">
+        <v>12114451</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>41518</v>
       </c>
-      <c r="B106">
-        <v>17052564</v>
-      </c>
-      <c r="C106">
-        <v>12176999</v>
+      <c r="B106" s="2">
+        <v>17007327</v>
+      </c>
+      <c r="C106" s="3">
+        <v>12133741</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>41548</v>
       </c>
-      <c r="B107">
-        <v>17075220</v>
-      </c>
-      <c r="C107">
-        <v>12207003</v>
+      <c r="B107" s="2">
+        <v>17027334</v>
+      </c>
+      <c r="C107" s="3">
+        <v>12156071</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>41579</v>
       </c>
-      <c r="B108">
-        <v>17104430</v>
-      </c>
-      <c r="C108">
-        <v>12239182</v>
+      <c r="B108" s="2">
+        <v>17055354</v>
+      </c>
+      <c r="C108" s="3">
+        <v>12183307</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>41609</v>
       </c>
-      <c r="B109">
-        <v>17139574</v>
-      </c>
-      <c r="C109">
-        <v>12271381</v>
+      <c r="B109" s="2">
+        <v>17090359</v>
+      </c>
+      <c r="C109" s="3">
+        <v>12214653</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>41640</v>
       </c>
-      <c r="B110">
-        <v>17178665</v>
-      </c>
-      <c r="C110">
-        <v>12301439</v>
+      <c r="B110" s="2">
+        <v>17130177</v>
+      </c>
+      <c r="C110" s="3">
+        <v>12247801</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>41671</v>
       </c>
-      <c r="B111">
-        <v>17218387</v>
-      </c>
-      <c r="C111">
-        <v>12328011</v>
+      <c r="B111" s="2">
+        <v>17171251</v>
+      </c>
+      <c r="C111" s="3">
+        <v>12279607</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>41699</v>
       </c>
-      <c r="B112">
-        <v>17255715</v>
-      </c>
-      <c r="C112">
-        <v>12351005</v>
+      <c r="B112" s="2">
+        <v>17209904</v>
+      </c>
+      <c r="C112" s="3">
+        <v>12307178</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>41730</v>
       </c>
-      <c r="B113">
-        <v>17290503</v>
-      </c>
-      <c r="C113">
-        <v>12372040</v>
+      <c r="B113" s="2">
+        <v>17244809</v>
+      </c>
+      <c r="C113" s="3">
+        <v>12329593</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>41760</v>
       </c>
-      <c r="B114">
-        <v>17326065</v>
-      </c>
-      <c r="C114">
-        <v>12393855</v>
+      <c r="B114" s="2">
+        <v>17278873</v>
+      </c>
+      <c r="C114" s="3">
+        <v>12348595</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>41791</v>
       </c>
-      <c r="B115">
-        <v>17365367</v>
-      </c>
-      <c r="C115">
-        <v>12418413</v>
+      <c r="B115" s="2">
+        <v>17315752</v>
+      </c>
+      <c r="C115" s="3">
+        <v>12366458</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>41821</v>
       </c>
-      <c r="B116">
-        <v>17406410</v>
-      </c>
-      <c r="C116">
-        <v>12445306</v>
+      <c r="B116" s="2">
+        <v>17355046</v>
+      </c>
+      <c r="C116" s="3">
+        <v>12383399</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>41852</v>
       </c>
-      <c r="B117">
-        <v>17446826</v>
-      </c>
-      <c r="C117">
-        <v>12473503</v>
+      <c r="B117" s="2">
+        <v>17396210</v>
+      </c>
+      <c r="C117" s="3">
+        <v>12399920</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>41883</v>
       </c>
-      <c r="B118">
-        <v>17484353</v>
-      </c>
-      <c r="C118">
-        <v>12501664</v>
+      <c r="B118" s="2">
+        <v>17437136</v>
+      </c>
+      <c r="C118" s="3">
+        <v>12415237</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>41913</v>
       </c>
-      <c r="B119">
-        <v>17517613</v>
-      </c>
-      <c r="C119">
-        <v>12528142</v>
+      <c r="B119" s="2">
+        <v>17475476</v>
+      </c>
+      <c r="C119" s="3">
+        <v>12427789</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>41944</v>
       </c>
-      <c r="B120">
-        <v>17545380</v>
-      </c>
-      <c r="C120">
-        <v>12551420</v>
+      <c r="B120" s="2">
+        <v>17509491</v>
+      </c>
+      <c r="C120" s="3">
+        <v>12436395</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>41974</v>
       </c>
-      <c r="B121">
-        <v>17566281</v>
-      </c>
-      <c r="C121">
-        <v>12570050</v>
+      <c r="B121" s="2">
+        <v>17539690</v>
+      </c>
+      <c r="C121" s="3">
+        <v>12441578</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>42005</v>
       </c>
-      <c r="B122">
-        <v>17620300</v>
-      </c>
-      <c r="C122">
-        <v>12600763</v>
+      <c r="B122" s="2">
+        <v>17567313</v>
+      </c>
+      <c r="C122" s="3">
+        <v>12444596</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>42036</v>
       </c>
-      <c r="B123">
-        <v>17667692</v>
-      </c>
-      <c r="C123">
-        <v>12620228</v>
+      <c r="B123" s="2">
+        <v>17594234</v>
+      </c>
+      <c r="C123" s="3">
+        <v>12446795</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>42064</v>
       </c>
-      <c r="B124">
-        <v>17712084</v>
-      </c>
-      <c r="C124">
-        <v>12614626</v>
+      <c r="B124" s="2">
+        <v>17623026</v>
+      </c>
+      <c r="C124" s="3">
+        <v>12449829</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>42095</v>
       </c>
-      <c r="B125">
-        <v>17754658</v>
-      </c>
-      <c r="C125">
-        <v>12596728</v>
+      <c r="B125" s="2">
+        <v>17652860</v>
+      </c>
+      <c r="C125" s="3">
+        <v>12454097</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="1"/>
+      <c r="A126" s="1">
+        <v>42125</v>
+      </c>
+      <c r="B126" s="2">
+        <v>17681771</v>
+      </c>
+      <c r="C126" s="3">
+        <v>12459177</v>
+      </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="1"/>
+      <c r="A127" s="1">
+        <v>42156</v>
+      </c>
+      <c r="B127" s="2">
+        <v>17707867</v>
+      </c>
+      <c r="C127" s="3">
+        <v>12464577</v>
+      </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A132" s="1"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A138" s="1"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A139" s="1"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A140" s="1"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A141" s="1"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A142" s="1"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A143" s="1"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A146" s="1"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A147" s="1"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A148" s="1"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A149" s="1"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A150" s="1"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A151" s="1"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A153" s="1"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A155" s="1"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A156" s="1"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A157" s="1"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A158" s="1"/>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A159" s="1"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A161" s="1"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A162" s="1"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A163" s="1"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A164" s="1"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A165" s="1"/>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A166" s="1"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A167" s="1"/>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A168" s="1"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A169" s="1"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A170" s="1"/>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A171" s="1"/>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A172" s="1"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A173" s="1"/>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A174" s="1"/>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A175" s="1"/>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A176" s="1"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A177" s="1"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A178" s="1"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A181" s="1"/>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A182" s="1"/>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A183" s="1"/>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A184" s="1"/>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A185" s="1"/>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A186" s="1"/>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A193" s="1"/>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A194" s="1"/>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A195" s="1"/>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A197" s="1"/>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A198" s="1"/>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A199" s="1"/>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A200" s="1"/>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A201" s="1"/>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A202" s="1"/>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A203" s="1"/>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A204" s="1"/>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A205" s="1"/>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A206" s="1"/>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A207" s="1"/>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A208" s="1"/>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A209" s="1"/>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A210" s="1"/>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A211" s="1"/>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A212" s="1"/>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A213" s="1"/>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A214" s="1"/>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A215" s="1"/>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A216" s="1"/>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A217" s="1"/>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A218" s="1"/>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A219" s="1"/>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A220" s="1"/>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A221" s="1"/>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A222" s="1"/>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A223" s="1"/>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A224" s="1"/>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A225" s="1"/>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A226" s="1"/>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A227" s="1"/>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A228" s="1"/>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A229" s="1"/>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A230" s="1"/>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A231" s="1"/>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A232" s="1"/>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A233" s="1"/>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A234" s="1"/>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A235" s="1"/>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A236" s="1"/>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A237" s="1"/>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A238" s="1"/>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A239" s="1"/>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A240" s="1"/>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A241" s="1"/>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A242" s="1"/>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A243" s="1"/>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A244" s="1"/>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A245" s="1"/>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A246" s="1"/>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A247" s="1"/>
+      <c r="A128" s="1">
+        <v>42186</v>
+      </c>
+      <c r="B128" s="2">
+        <v>17732005</v>
+      </c>
+      <c r="C128" s="3">
+        <v>12470907</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="1">
+        <v>42217</v>
+      </c>
+      <c r="B129" s="2">
+        <v>17755703</v>
+      </c>
+      <c r="C129" s="3">
+        <v>12479250</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" s="1">
+        <v>42248</v>
+      </c>
+      <c r="B130" s="2">
+        <v>17781478</v>
+      </c>
+      <c r="C130" s="3">
+        <v>12491443</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="1">
+        <v>42278</v>
+      </c>
+      <c r="B131" s="2">
+        <v>17811077</v>
+      </c>
+      <c r="C131" s="3">
+        <v>12508657</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B132" s="2">
+        <v>17843829</v>
+      </c>
+      <c r="C132" s="3">
+        <v>12529472</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="1">
+        <v>42339</v>
+      </c>
+      <c r="B133" s="2">
+        <v>17877530</v>
+      </c>
+      <c r="C133" s="3">
+        <v>12550977</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="1">
+        <v>42370</v>
+      </c>
+      <c r="B134" s="2">
+        <v>17908829</v>
+      </c>
+      <c r="C134" s="3">
+        <v>12570214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" s="1">
+        <v>42401</v>
+      </c>
+      <c r="B135" s="2">
+        <v>17935995</v>
+      </c>
+      <c r="C135" s="3">
+        <v>12585518</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="1">
+        <v>42430</v>
+      </c>
+      <c r="B136" s="2">
+        <v>17959318</v>
+      </c>
+      <c r="C136" s="3">
+        <v>12596876</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" s="1">
+        <v>42461</v>
+      </c>
+      <c r="B137" s="2">
+        <v>17982086</v>
+      </c>
+      <c r="C137" s="3">
+        <v>12606014</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B138" s="2">
+        <v>18008236</v>
+      </c>
+      <c r="C138" s="3">
+        <v>12615703</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="1">
+        <v>42522</v>
+      </c>
+      <c r="B139" s="2">
+        <v>18038968</v>
+      </c>
+      <c r="C139" s="3">
+        <v>12628206</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B140" s="2">
+        <v>18071628</v>
+      </c>
+      <c r="C140" s="3">
+        <v>12644405</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="1">
+        <v>42583</v>
+      </c>
+      <c r="B141" s="2">
+        <v>18101817</v>
+      </c>
+      <c r="C141" s="3">
+        <v>12662762</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B142" s="2">
+        <v>18126351</v>
+      </c>
+      <c r="C142" s="3">
+        <v>12680821</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B143" s="2">
+        <v>18144705</v>
+      </c>
+      <c r="C143" s="3">
+        <v>12697343</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="1">
+        <v>42675</v>
+      </c>
+      <c r="B144" s="2">
+        <v>18157698</v>
+      </c>
+      <c r="C144" s="3">
+        <v>12711707</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B145" s="2">
+        <v>18165425</v>
+      </c>
+      <c r="C145" s="3">
+        <v>12723289</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B146" s="2">
+        <v>18175914</v>
+      </c>
+      <c r="C146" s="3">
+        <v>12757792</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" s="1">
+        <v>42767</v>
+      </c>
+      <c r="B147" s="2">
+        <v>18189592</v>
+      </c>
+      <c r="C147" s="3">
+        <v>12799028</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" s="1">
+        <v>42795</v>
+      </c>
+      <c r="B148" s="2">
+        <v>18226929</v>
+      </c>
+      <c r="C148" s="3">
+        <v>12842576</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="1">
+        <v>42826</v>
+      </c>
+      <c r="B149" s="2">
+        <v>18254693</v>
+      </c>
+      <c r="C149" s="3">
+        <v>12872464</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>